<commit_message>
final edits for revisions
</commit_message>
<xml_diff>
--- a/inVitroAnalysis/GrowthCurves/LoperamideGrowthCurves_20220523.xlsx
+++ b/inVitroAnalysis/GrowthCurves/LoperamideGrowthCurves_20220523.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstevick/Documents/Research/LoperamideMicrobiota/Loperamide_GrowthCurves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstevick/Documents/Research/LoperamideMicrobiota/Repo_LoperamideZebrafishDysbiosis/inVitroAnalysis/GrowthCurves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E30C06-869C-924B-9D42-017AB67C4ECC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EA1514-648E-2C47-AC91-B33CBC55C88A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9860" yWindow="11100" windowWidth="27640" windowHeight="16080" activeTab="1" xr2:uid="{23DC0291-A993-8648-9AFC-36030E572DDE}"/>
   </bookViews>
@@ -1978,7 +1978,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>